<commit_message>
18/08/02 this is how we work? 18/08/02 this is how we work? 18/08/02 this is how we work? 18/08/02 this is how we work? 18/08/02 this is how we work? 18/08/02 this is how we work? 18/08/02 this is how we work? 18/08/02 this is how we work? 18/08/02 this is how we work? 18/08/02 this is how we work? 18/08/02 this is how we work? 18/08/02 this is how we work? 18/08/02 this is how we work? 18/08/02 this is how we work? 18/08/02 this is how we work? 18/08/02 this is how we work? 18/08/02 this is how we work? 18/08/02 this is how we work?
</commit_message>
<xml_diff>
--- a/datamodel.xlsx
+++ b/datamodel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joohyun/Desktop/Developer/MyGit/moonglow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{48363643-5D31-0245-B7C2-C942203C5805}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{631CBDD2-6548-E542-BFE8-84556BE7DCD2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1620" yWindow="1580" windowWidth="25000" windowHeight="14240" xr2:uid="{BEE499A2-0539-CC47-8733-5ED594D19776}"/>
   </bookViews>
@@ -25,46 +25,83 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>종목코드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>종가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>시가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>저가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>고가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>거래량</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>기관순매매</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>외국인순매매</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>거래일</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>논리명</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>물리명</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>인포타입</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이터타입</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 일간시세</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 관심종목</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
@@ -80,12 +117,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -102,8 +145,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -420,42 +472,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32CA62F3-8BC3-B148-8225-7BAE190C59C4}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J2" t="s">
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>